<commit_message>
[Contacts] - Contacts partenaires handled
</commit_message>
<xml_diff>
--- a/neo4j/ressources/2021 PLANETE SOLIDAIRE - CONTACTS PARTENAIRES.xlsx
+++ b/neo4j/ressources/2021 PLANETE SOLIDAIRE - CONTACTS PARTENAIRES.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studisg-my.sharepoint.com/personal/caroline_depaoli_isg_fr/Documents/EMS/Annee 2020-2021/Projets entrepreneuriaux premier cycle/Planete solidaire 2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mngen\Downloads\python_ice\neo4j\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_8A0672A81D5CEE319002A62FF4473BDC3648C20B" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6417F3E-4335-4FDB-B7D9-20C409DBF9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Partenaire</t>
   </si>
@@ -66,9 +66,6 @@
     <t>srlauredumas@yahoo.fr</t>
   </si>
   <si>
-    <t>Groupe Pic</t>
-  </si>
-  <si>
     <t>Sinapian</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t xml:space="preserve">david.sinapian@groupe-pic.com </t>
   </si>
   <si>
-    <t>Daily Pic</t>
-  </si>
-  <si>
     <t>Etienne</t>
   </si>
   <si>
@@ -93,30 +87,9 @@
     <t xml:space="preserve">lilian.etienne@dailypic.com </t>
   </si>
   <si>
-    <t>Pauline</t>
-  </si>
-  <si>
-    <t>Monot</t>
-  </si>
-  <si>
     <t>DG</t>
   </si>
   <si>
-    <t xml:space="preserve">pauline.monot@groupe-pic.com </t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Terrier</t>
-  </si>
-  <si>
-    <t>Chargée de com</t>
-  </si>
-  <si>
-    <t>charlotte.terrier@groupe-pic.com</t>
-  </si>
-  <si>
     <t>Mama Shelter</t>
   </si>
   <si>
@@ -132,21 +105,6 @@
     <t>serge@mamashelter.com</t>
   </si>
   <si>
-    <t>Vincent</t>
-  </si>
-  <si>
-    <t>Brun</t>
-  </si>
-  <si>
-    <t>Chef marketing com</t>
-  </si>
-  <si>
-    <t>vincent.brun@mamashelter.com</t>
-  </si>
-  <si>
-    <t>Chateau La Brande</t>
-  </si>
-  <si>
     <t>Maude</t>
   </si>
   <si>
@@ -162,9 +120,6 @@
     <t>+ 33 (0)6 83 72 46 60</t>
   </si>
   <si>
-    <t>Oui Chef</t>
-  </si>
-  <si>
     <t>Rutger</t>
   </si>
   <si>
@@ -186,9 +141,6 @@
     <t>tom.chauvet@isg.fr</t>
   </si>
   <si>
-    <t>Les arcs</t>
-  </si>
-  <si>
     <t>Marine</t>
   </si>
   <si>
@@ -204,24 +156,9 @@
     <t>(0)6 72 32 66 87</t>
   </si>
   <si>
-    <t>Village Pro BTP</t>
-  </si>
-  <si>
-    <t>Stéphane</t>
-  </si>
-  <si>
     <t>Besnier</t>
   </si>
   <si>
-    <t>Esprit de voyages</t>
-  </si>
-  <si>
-    <t>Signé Toqué</t>
-  </si>
-  <si>
-    <t>Ristorante Duomo</t>
-  </si>
-  <si>
     <t>A la découverte des langues</t>
   </si>
   <si>
@@ -237,20 +174,44 @@
     <t>humblot27@wanadoo.fr</t>
   </si>
   <si>
-    <t>Artiste</t>
-  </si>
-  <si>
     <t>François</t>
   </si>
   <si>
     <t>Dumas</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Artiste Dumas</t>
+  </si>
+  <si>
+    <t>Groupe PIC</t>
+  </si>
+  <si>
+    <t>Daily PIC</t>
+  </si>
+  <si>
+    <t>Oui Chef!</t>
+  </si>
+  <si>
+    <t>Les Arcs</t>
+  </si>
+  <si>
+    <t>Villages Pro BTP</t>
+  </si>
+  <si>
+    <t>Château LaBrande</t>
+  </si>
+  <si>
+    <t>Stéphanie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,21 +545,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -618,77 +580,95 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -696,167 +676,128 @@
       <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
       <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -864,15 +805,12 @@
     <hyperlink ref="E2" r:id="rId1" display="mailto:srlauredumas@yahoo.fr" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E3" r:id="rId2" display="mailto:david.sinapian@groupe-pic.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E4" r:id="rId3" display="mailto:lilian.etienne@dailypic.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" display="mailto:pauline.monot@groupe-pic.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" display="mailto:charlotte.terrier@groupe-pic.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId6" display="mailto:serge@mamashelter.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E8" r:id="rId7" display="mailto:vincent.brun@mamashelter.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E12" r:id="rId10" display="mailto:m.ruas@bourgsaintmaurice.fr" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E9" r:id="rId6" display="mailto:m.ruas@bourgsaintmaurice.fr" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E5" r:id="rId9" display="mailto:serge@mamashelter.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -885,15 +823,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010043CE4E1FA2FCB14FB9B7112BF7A3D4BF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ab722eb03a140c46b957100d7ec1ae3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9e00ab22-e255-43f5-ae0e-51305c57963a" xmlns:ns4="91e831ff-3009-4d57-bde4-43a3b81f56c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3657ec7d0a2f1f05179f19e0a91e452f" ns3:_="" ns4:_="">
     <xsd:import namespace="9e00ab22-e255-43f5-ae0e-51305c57963a"/>
@@ -1116,14 +1045,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7052C47A-F4DC-443C-B6D8-D7B63511CEEF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7052C47A-F4DC-443C-B6D8-D7B63511CEEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D160F04-25EA-4C36-BEA1-20755F17CFF9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C3C2CDD-B38F-452F-84C9-C3FC3170A90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9e00ab22-e255-43f5-ae0e-51305c57963a"/>
+    <ds:schemaRef ds:uri="91e831ff-3009-4d57-bde4-43a3b81f56c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C3C2CDD-B38F-452F-84C9-C3FC3170A90B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D160F04-25EA-4C36-BEA1-20755F17CFF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>